<commit_message>
Updated documentation and added mobile application skeleton (#4)
* Updated documentation

* Updated .NET version

* Updated documentation and added application skeleton
</commit_message>
<xml_diff>
--- a/docs/ExportedEstimate.xlsx
+++ b/docs/ExportedEstimate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Microsoft Azure Estimate</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Estimated upfront cost</t>
   </si>
   <si>
+    <t>Databases</t>
+  </si>
+  <si>
     <t>Azure SQL Database</t>
   </si>
   <si>
@@ -53,10 +56,16 @@
     <t xml:space="preserve">Single Database, DTU Purchase Model, Basic Tier, B: 5 DTUs, 2 GB included storage per DB, 1 Database(s) x 730 Hours, 0 GB Storage, 0 GB Point-In-Time Restore, RA-GRS Backup Storage Redundancy,  0 x 5 GB Long Term Retention</t>
   </si>
   <si>
+    <t>Storage</t>
+  </si>
+  <si>
     <t>Storage Accounts</t>
   </si>
   <si>
     <t>Block Blob Storage, General Purpose V2, Hierarchical Namespace, LRS Redundancy, Hot Access Tier, 10 GB Capacity - Pay as you go, 10 x 10,000 Write operations, 10 x 10,000 Read operations, 10 x 10,000 Iterative Read operations, 10 x 100 Iterative Write operations, 1,000 GB Data Retrieval, 1,000 GB Data Write, 10 GB Index, 1 x 10,000 Other operations</t>
+  </si>
+  <si>
+    <t>Containers</t>
   </si>
   <si>
     <t>Azure Container Apps</t>
@@ -71,10 +80,22 @@
     <t xml:space="preserve">Basic Tier, 1 registries x 30 days,   0 GB Extra Storage, Container Build - 1 CPUs x 12000 Seconds - Internet Egress transfer type, 5 GB outbound data transfer from East US routed via Microsoft Global Network</t>
   </si>
   <si>
+    <t>Developer tools</t>
+  </si>
+  <si>
     <t>Azure DevOps</t>
   </si>
   <si>
     <t>2 Basic Plan license users, 0 Basic + Test Plans license users, Free tier - 1 Microsoft Hosted Pipeline(s), 1 Self Hosted Pipeline(s), 0 GB Artifacts</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Notification Hubs</t>
+  </si>
+  <si>
+    <t>Free tier</t>
   </si>
   <si>
     <t>Support</t>
@@ -101,7 +122,7 @@
     <t>All prices shown are in United States – Dollar ($) USD. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 10/5/2023 5:04:34 AM UTC.</t>
+    <t>This estimate was created at 10/6/2023 11:59:44 PM UTC.</t>
   </si>
 </sst>
 </file>
@@ -358,18 +379,20 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5">
         <v>4.89708333333334</v>
@@ -398,18 +421,20 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5">
         <v>1.915</v>
@@ -438,18 +463,20 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
@@ -478,18 +505,20 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5">
         <v>5.598</v>
@@ -518,16 +547,18 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -557,14 +588,20 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="13" t="s">
-        <v>21</v>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="5">
         <v>0</v>
       </c>
@@ -592,17 +629,21 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>23</v>
+      <c r="E10" s="12"/>
+      <c r="F10" s="5">
+        <v>0</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -628,10 +669,10 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="13" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -660,10 +701,10 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="13" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -691,16 +732,14 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="14" t="s">
-        <v>26</v>
+      <c r="D13" s="13" t="s">
+        <v>32</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="15">
-        <v>12.41008333333334</v>
+      <c r="E13" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -725,10 +764,16 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="15">
+        <v>12.41008333333334</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -750,9 +795,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -780,15 +823,15 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>28</v>
+      <c r="A16" s="13" t="s">
+        <v>34</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="7"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -811,7 +854,7 @@
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -840,7 +883,9 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="16"/>
+      <c r="A18" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -868,13 +913,13 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
       <c r="H19" s="7"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -28367,8 +28412,8 @@
   <mergeCells>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A16:G16"/>
     <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>